<commit_message>
fix bug in SE
</commit_message>
<xml_diff>
--- a/inst/extdata/socio_economic/socio_economic_input_heavy.xlsx
+++ b/inst/extdata/socio_economic/socio_economic_input_heavy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattj\Dropbox\Projects\EN2691 CEPopMod\main\CEMPRA\inst\extdata\socio_economic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484E0B3C-2F22-49F6-BC28-381A6E4461A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792EED0D-0EFF-4A46-90DC-C0E9CAB2B1D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="516" windowWidth="23256" windowHeight="12456" tabRatio="699" xr2:uid="{1AD852B4-9C7D-474C-A280-4470E2592A52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="699" activeTab="1" xr2:uid="{1AD852B4-9C7D-474C-A280-4470E2592A52}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Actions" sheetId="1" r:id="rId1"/>
@@ -8138,7 +8138,7 @@
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -8481,8 +8481,8 @@
   </sheetPr>
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8562,10 +8562,10 @@
         <v>km</v>
       </c>
       <c r="E3" s="3">
-        <v>0.35</v>
+        <v>0.5</v>
       </c>
       <c r="F3" s="3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="G3" s="3">
         <v>0.2</v>
@@ -8595,10 +8595,10 @@
         <v>km</v>
       </c>
       <c r="E4" s="3">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="3">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="G4" s="3">
         <v>0.05</v>
@@ -8631,7 +8631,7 @@
         <v>30</v>
       </c>
       <c r="F5" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G5" s="3">
         <v>0</v>
@@ -8664,7 +8664,7 @@
         <v>2000</v>
       </c>
       <c r="F6" s="9">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G6" s="9">
         <v>500</v>
@@ -8694,10 +8694,10 @@
         <v>m²</v>
       </c>
       <c r="E7" s="9">
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="F7" s="9">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="G7" s="9">
         <v>5000</v>
@@ -8730,7 +8730,7 @@
         <v>300</v>
       </c>
       <c r="F8" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -8763,7 +8763,7 @@
         <v>300</v>
       </c>
       <c r="F9" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -9887,6 +9887,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006256975931115C42B154129ACF64F69B" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8760ac783ae80450fdcfd00892bf61e3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8739a20a3ebaa886781928d73ec2eaf7" ns3:_="">
     <xsd:import namespace="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
@@ -10030,22 +10045,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72DE81FF-AA4E-454F-9486-E6DCC5C8CF30}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA07873-0FD5-45A1-B17B-248E491F3F34}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{28B5C721-92D3-4BD7-B3B7-E31C54E2EC22}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10061,28 +10085,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CA07873-0FD5-45A1-B17B-248E491F3F34}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{72DE81FF-AA4E-454F-9486-E6DCC5C8CF30}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="40ccca9c-0b7e-4ba6-a758-0e8a1fa03b03"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>